<commit_message>
#1102 - Create action logic
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689AA532-EFF5-46BF-998D-F15A9FB9A96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB46E0E-92A6-4DB8-A7D5-D2EBFF1A09A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -29,23 +29,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="200">
   <si>
     <t>Cell Colors</t>
   </si>
@@ -598,15 +587,9 @@
     <t>Add a copy of "Submission of "Draft" Initial Project Description" to thisPhase at thisEventACTUAL +14</t>
   </si>
   <si>
-    <t>{"phase_name":"Project Notification Review","work_type_id": 1, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Project Notification" }</t>
-  </si>
-  <si>
     <t>Add a copy of "Initial Review of "Draft" Initial Project Description" to thisPhase at thisEventACTUAL +21</t>
   </si>
   <si>
-    <t>{"phase_name":"Project Notification Review","work_type_id": 1, "ea_act_id": 3, "event_name": "\"Draft\" Project Notification Initial Review" }</t>
-  </si>
-  <si>
     <t>SetPhasesStatus</t>
   </si>
   <si>
@@ -815,6 +798,15 @@
   </si>
   <si>
     <t>{"work_state": "COMPLETED"}</t>
+  </si>
+  <si>
+    <t>{"start_date_locked": true}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Project Notification Review","work_type_id": 1, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Project Notification", "start_at": 14 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Project Notification Review","work_type_id": 1, "ea_act_id": 3, "event_name": "\"Draft\" Project Notification Initial Review", "start_at": 21 }</t>
   </si>
 </sst>
 </file>
@@ -1378,55 +1370,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1447,18 +1439,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1484,7 +1476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1510,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1536,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1562,226 +1554,226 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93"/>
     </row>
   </sheetData>
@@ -1824,22 +1816,22 @@
       <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1880,7 +1872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1919,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1958,7 +1950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1997,7 +1989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2036,7 +2028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2075,7 +2067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2114,7 +2106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2153,7 +2145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2192,7 +2184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2231,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2270,7 +2262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2312,7 +2304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2354,7 +2346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2396,7 +2388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2438,7 +2430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2477,7 +2469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2516,7 +2508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2558,7 +2550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2597,7 +2589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2639,7 +2631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2681,7 +2673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2723,7 +2715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2765,7 +2757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2804,7 +2796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2843,7 +2835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2882,7 +2874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2924,7 +2916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2966,7 +2958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3005,7 +2997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3047,7 +3039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3089,7 +3081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3128,7 +3120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3170,7 +3162,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3212,7 +3204,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3251,7 +3243,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3293,7 +3285,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3335,7 +3327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3374,7 +3366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3416,7 +3408,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3458,7 +3450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3497,7 +3489,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3539,7 +3531,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3581,7 +3573,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3620,7 +3612,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3659,7 +3651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3698,7 +3690,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3737,7 +3729,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3779,7 +3771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3818,7 +3810,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3857,7 +3849,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3899,7 +3891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3941,7 +3933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3980,7 +3972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4022,7 +4014,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4064,7 +4056,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4103,7 +4095,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4145,7 +4137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4187,7 +4179,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4226,7 +4218,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4268,7 +4260,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4310,7 +4302,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4349,7 +4341,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4391,7 +4383,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4433,7 +4425,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4472,7 +4464,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4511,7 +4503,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4553,7 +4545,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4656,16 +4648,16 @@
       <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4682,7 +4674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4700,7 +4692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4718,7 +4710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4736,7 +4728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4754,7 +4746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4772,7 +4764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4790,7 +4782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4808,7 +4800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4826,7 +4818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4844,7 +4836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4862,7 +4854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4880,7 +4872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4898,7 +4890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4916,7 +4908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4956,25 +4948,25 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="176.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="131.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="176.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="141.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4997,7 +4989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5021,7 +5013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -5039,13 +5031,13 @@
         <v>125</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>126</v>
+        <v>198</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -5060,16 +5052,16 @@
         <v>124</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>128</v>
+        <v>199</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -5081,19 +5073,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -5105,19 +5097,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -5129,19 +5121,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5153,19 +5145,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5177,19 +5169,19 @@
         <v>Starts the "clock" for Project Notification</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -5201,19 +5193,19 @@
         <v>Minister is delegated to make the final Project Notification Decision</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -5225,19 +5217,19 @@
         <v>CEAO is delegated to make the final Project Notification Decision</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -5249,19 +5241,19 @@
         <v>Days are added to the PHASE END EVENT</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -5273,19 +5265,19 @@
         <v>Days are added to the PHASE END EVENT</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -5297,19 +5289,19 @@
         <v>Days are added to the PHASE END EVENT</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -5321,19 +5313,19 @@
         <v>Days are added to the PHASE END EVENT</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -5345,19 +5337,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -5369,19 +5361,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -5393,19 +5385,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -5417,19 +5409,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -5441,19 +5433,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -5465,19 +5457,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5489,19 +5481,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5513,19 +5505,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -5537,19 +5529,19 @@
         <v>No Further Review Required</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G24" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -5561,19 +5553,19 @@
         <v>No Further Review Required</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -5585,19 +5577,19 @@
         <v>More Information Needed</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -5609,19 +5601,19 @@
         <v>More Information Needed</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -5633,19 +5625,19 @@
         <v>More Information Needed</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -5657,19 +5649,19 @@
         <v>Project Referred to Minister (s.11)</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -5681,19 +5673,19 @@
         <v>Project Referred to Minister (s.11)</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G30" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -5705,19 +5697,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="G31" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -5729,19 +5721,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G32" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5753,19 +5745,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G33" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5777,19 +5769,19 @@
         <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G34" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5801,19 +5793,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="G35" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -5825,19 +5817,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G36" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -5849,19 +5841,19 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="G37" s="3">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -5873,28 +5865,28 @@
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G38" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D42"/>
     </row>
   </sheetData>
@@ -5924,41 +5916,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.88671875" style="4"/>
-    <col min="60" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.85546875" style="4"/>
+    <col min="60" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1" t="s">
@@ -5967,11 +5959,11 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="1" t="s">
@@ -5983,11 +5975,11 @@
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -6030,7 +6022,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -6053,7 +6045,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>36</v>
@@ -6062,12 +6054,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F4" s="2" t="b">
         <v>0</v>
@@ -6085,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>39</v>
@@ -6094,49 +6086,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>35</v>
@@ -6148,12 +6140,12 @@
         <v>54</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>35</v>
@@ -6165,29 +6157,29 @@
         <v>76</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>81</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>35</v>
@@ -6196,12 +6188,12 @@
         <v>38</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>35</v>
@@ -6211,9 +6203,9 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>35</v>
@@ -6223,9 +6215,9 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>76</v>
@@ -6235,9 +6227,9 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>76</v>
@@ -6247,9 +6239,9 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>81</v>
@@ -6259,7 +6251,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
@@ -6270,15 +6262,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="4" t="s">
         <v>42</v>
       </c>
@@ -6286,7 +6278,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="4" t="s">
         <v>42</v>
       </c>
@@ -6294,15 +6286,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="4" t="s">
         <v>42</v>
       </c>
@@ -6310,7 +6302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="4" t="s">
         <v>42</v>
       </c>
@@ -6318,23 +6310,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H24" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H25" s="4" t="s">
         <v>42</v>
       </c>
@@ -6342,7 +6334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H26" s="4" t="s">
         <v>54</v>
       </c>
@@ -6350,7 +6342,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="4" t="s">
         <v>54</v>
       </c>
@@ -6358,7 +6350,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H28" s="4" t="s">
         <v>54</v>
       </c>
@@ -6366,7 +6358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H29" s="4" t="s">
         <v>54</v>
       </c>
@@ -6374,7 +6366,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H30" s="4" t="s">
         <v>57</v>
       </c>
@@ -6382,7 +6374,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H31" s="4" t="s">
         <v>57</v>
       </c>
@@ -6390,23 +6382,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H32" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="4" t="s">
         <v>57</v>
       </c>
@@ -6414,41 +6406,41 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H36" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I36" s="2" t="s">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H37" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H38" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
#1102 - Create action logic (#1144)
* suspension/resumption

* actions

* suspension/resumption

* implement actions - initial

* #1102 - Create action logic

---------

Co-authored-by: Dinesh <dinesh.pb@aot-technologies.com>
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2492B43-4F45-43D3-979F-E51D75366409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB46E0E-92A6-4DB8-A7D5-D2EBFF1A09A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -28,17 +28,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1381,55 +1370,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1450,18 +1439,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1513,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1539,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1565,226 +1554,226 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93"/>
     </row>
   </sheetData>
@@ -1824,25 +1813,25 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1883,7 +1872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1922,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1961,7 +1950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2000,7 +1989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2039,7 +2028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2078,7 +2067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2117,7 +2106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2156,7 +2145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2195,7 +2184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2234,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2273,7 +2262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2315,7 +2304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2357,7 +2346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2399,7 +2388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2441,7 +2430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2480,7 +2469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2519,7 +2508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2561,7 +2550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2600,7 +2589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2642,7 +2631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2684,7 +2673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2726,7 +2715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2768,7 +2757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2807,7 +2796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2846,7 +2835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2885,7 +2874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2927,7 +2916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2969,7 +2958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3008,7 +2997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3050,7 +3039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3092,7 +3081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3131,7 +3120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3173,7 +3162,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3215,7 +3204,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3254,7 +3243,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3296,7 +3285,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3338,7 +3327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3377,7 +3366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3419,7 +3408,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3461,7 +3450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3500,7 +3489,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3542,7 +3531,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3584,7 +3573,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3623,7 +3612,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3662,7 +3651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3701,7 +3690,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3740,7 +3729,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3782,7 +3771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3821,7 +3810,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3860,7 +3849,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3902,7 +3891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3944,7 +3933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3983,7 +3972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4025,7 +4014,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4067,7 +4056,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4106,7 +4095,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4148,7 +4137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4190,7 +4179,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4229,7 +4218,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4271,7 +4260,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4313,7 +4302,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4352,7 +4341,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4394,7 +4383,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4436,7 +4425,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4475,7 +4464,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4514,7 +4503,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4556,7 +4545,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4656,19 +4645,19 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4685,7 +4674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4703,7 +4692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4721,7 +4710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4739,7 +4728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4757,7 +4746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4775,7 +4764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4793,7 +4782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4811,7 +4800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4829,7 +4818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4847,7 +4836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4865,7 +4854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4883,7 +4872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4901,7 +4890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4919,7 +4908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4959,25 +4948,25 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="176.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="140" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="176.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="141.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -5000,7 +4989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5024,7 +5013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -5048,7 +5037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -5072,7 +5061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -5096,7 +5085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -5120,7 +5109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -5144,7 +5133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5168,7 +5157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5192,7 +5181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -5216,7 +5205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -5240,7 +5229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -5264,7 +5253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -5288,7 +5277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -5312,7 +5301,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -5336,7 +5325,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -5360,7 +5349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -5384,7 +5373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -5408,7 +5397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -5432,7 +5421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -5456,7 +5445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -5480,7 +5469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5504,7 +5493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5528,7 +5517,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -5552,7 +5541,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -5576,7 +5565,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -5600,7 +5589,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -5624,7 +5613,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -5648,7 +5637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -5672,7 +5661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -5696,7 +5685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -5720,7 +5709,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -5744,7 +5733,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5768,7 +5757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5792,7 +5781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5816,7 +5805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -5840,7 +5829,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -5864,7 +5853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -5888,16 +5877,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D42"/>
     </row>
   </sheetData>
@@ -5927,34 +5916,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.88671875" style="4"/>
-    <col min="60" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.85546875" style="4"/>
+    <col min="60" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -6033,7 +6022,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -6065,7 +6054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>161</v>
       </c>
@@ -6097,7 +6086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>164</v>
       </c>
@@ -6120,7 +6109,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>168</v>
       </c>
@@ -6137,7 +6126,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>172</v>
       </c>
@@ -6154,7 +6143,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>174</v>
       </c>
@@ -6171,7 +6160,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>176</v>
       </c>
@@ -6188,7 +6177,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>179</v>
       </c>
@@ -6202,7 +6191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>181</v>
       </c>
@@ -6214,7 +6203,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>182</v>
       </c>
@@ -6226,7 +6215,7 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>183</v>
       </c>
@@ -6238,7 +6227,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>184</v>
       </c>
@@ -6250,7 +6239,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>185</v>
       </c>
@@ -6262,7 +6251,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
@@ -6273,7 +6262,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="4" t="s">
         <v>42</v>
       </c>
@@ -6281,7 +6270,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="4" t="s">
         <v>42</v>
       </c>
@@ -6289,7 +6278,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="4" t="s">
         <v>42</v>
       </c>
@@ -6297,7 +6286,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="4" t="s">
         <v>42</v>
       </c>
@@ -6305,7 +6294,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="4" t="s">
         <v>42</v>
       </c>
@@ -6313,7 +6302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="4" t="s">
         <v>42</v>
       </c>
@@ -6321,7 +6310,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="4" t="s">
         <v>42</v>
       </c>
@@ -6329,7 +6318,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H24" s="4" t="s">
         <v>42</v>
       </c>
@@ -6337,7 +6326,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H25" s="4" t="s">
         <v>42</v>
       </c>
@@ -6345,7 +6334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H26" s="4" t="s">
         <v>54</v>
       </c>
@@ -6353,7 +6342,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="4" t="s">
         <v>54</v>
       </c>
@@ -6361,7 +6350,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H28" s="4" t="s">
         <v>54</v>
       </c>
@@ -6369,7 +6358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H29" s="4" t="s">
         <v>54</v>
       </c>
@@ -6377,7 +6366,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H30" s="4" t="s">
         <v>57</v>
       </c>
@@ -6385,7 +6374,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H31" s="4" t="s">
         <v>57</v>
       </c>
@@ -6393,7 +6382,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H32" s="4" t="s">
         <v>57</v>
       </c>
@@ -6401,7 +6390,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="4" t="s">
         <v>57</v>
       </c>
@@ -6409,7 +6398,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="4" t="s">
         <v>57</v>
       </c>
@@ -6417,7 +6406,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" s="4" t="s">
         <v>170</v>
       </c>
@@ -6425,7 +6414,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36" s="4" t="s">
         <v>170</v>
       </c>
@@ -6433,7 +6422,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37" s="4" t="s">
         <v>170</v>
       </c>
@@ -6441,7 +6430,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38" s="4" t="s">
         <v>170</v>
       </c>
@@ -6449,7 +6438,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39" s="4" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
minister & ceao designation (#1151)
* minister & ceao designation

* additional parameter chagnes to templates
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\project_notification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB46E0E-92A6-4DB8-A7D5-D2EBFF1A09A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935D0CA8-2159-46F6-A5C5-4F6BE19AA8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -24,10 +24,21 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Events!$A$1:$M$68</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1370,55 +1381,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1439,18 +1450,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1476,7 +1487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1502,7 +1513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1528,7 +1539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1554,226 +1565,226 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93"/>
     </row>
   </sheetData>
@@ -1816,22 +1827,22 @@
       <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1872,7 +1883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1911,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1950,7 +1961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1989,7 +2000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2028,7 +2039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2067,7 +2078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2106,7 +2117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2145,7 +2156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2184,7 +2195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2223,7 +2234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2262,7 +2273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2304,7 +2315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2346,7 +2357,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2388,7 +2399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2430,7 +2441,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2469,7 +2480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2508,7 +2519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2550,7 +2561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2589,7 +2600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2631,7 +2642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2673,7 +2684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2715,7 +2726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2757,7 +2768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2796,7 +2807,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2835,7 +2846,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2874,7 +2885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2916,7 +2927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2958,7 +2969,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2997,7 +3008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3039,7 +3050,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3081,7 +3092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3120,7 +3131,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3162,7 +3173,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3204,7 +3215,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3243,7 +3254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3285,7 +3296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3327,7 +3338,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3366,7 +3377,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3408,7 +3419,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3450,7 +3461,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3489,7 +3500,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3531,7 +3542,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3573,7 +3584,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3612,7 +3623,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3651,7 +3662,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3690,7 +3701,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3729,7 +3740,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3771,7 +3782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3810,7 +3821,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3849,7 +3860,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3891,7 +3902,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3933,7 +3944,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3972,7 +3983,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4014,7 +4025,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4056,7 +4067,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4095,7 +4106,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4137,7 +4148,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4179,7 +4190,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4218,7 +4229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4260,7 +4271,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4302,7 +4313,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4341,7 +4352,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4383,7 +4394,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4425,7 +4436,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4464,7 +4475,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4503,7 +4514,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4545,7 +4556,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4648,16 +4659,16 @@
       <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4674,7 +4685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4692,7 +4703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4710,7 +4721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4728,7 +4739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4746,7 +4757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4764,7 +4775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4782,7 +4793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4800,7 +4811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4818,7 +4829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4836,7 +4847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4854,7 +4865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4872,7 +4883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4890,7 +4901,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4908,7 +4919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4948,25 +4959,25 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="176.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="141.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="176.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="141.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4989,7 +5000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5013,7 +5024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -5037,7 +5048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -5061,7 +5072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -5085,7 +5096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -5109,7 +5120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -5133,7 +5144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5157,7 +5168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5181,7 +5192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -5205,7 +5216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -5229,7 +5240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -5253,7 +5264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -5277,7 +5288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -5301,7 +5312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -5325,7 +5336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -5349,7 +5360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -5373,7 +5384,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -5397,7 +5408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -5421,7 +5432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -5445,7 +5456,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -5469,7 +5480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5493,7 +5504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5517,7 +5528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -5541,7 +5552,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -5565,7 +5576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -5589,7 +5600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -5613,7 +5624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -5637,7 +5648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -5661,7 +5672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -5685,7 +5696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -5709,7 +5720,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -5733,7 +5744,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5757,7 +5768,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5781,7 +5792,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5805,7 +5816,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -5829,7 +5840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -5853,7 +5864,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -5877,16 +5888,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D42"/>
     </row>
   </sheetData>
@@ -5916,34 +5927,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.85546875" style="4"/>
-    <col min="60" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.88671875" style="4"/>
+    <col min="60" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -6022,7 +6033,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -6054,7 +6065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>161</v>
       </c>
@@ -6086,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>164</v>
       </c>
@@ -6109,7 +6120,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>168</v>
       </c>
@@ -6126,7 +6137,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>172</v>
       </c>
@@ -6143,7 +6154,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>174</v>
       </c>
@@ -6160,7 +6171,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>176</v>
       </c>
@@ -6177,7 +6188,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>179</v>
       </c>
@@ -6191,7 +6202,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>181</v>
       </c>
@@ -6203,7 +6214,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>182</v>
       </c>
@@ -6215,7 +6226,7 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>183</v>
       </c>
@@ -6227,7 +6238,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>184</v>
       </c>
@@ -6239,7 +6250,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>185</v>
       </c>
@@ -6251,7 +6262,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
@@ -6262,7 +6273,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="4" t="s">
         <v>42</v>
       </c>
@@ -6270,7 +6281,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="4" t="s">
         <v>42</v>
       </c>
@@ -6278,7 +6289,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="4" t="s">
         <v>42</v>
       </c>
@@ -6286,7 +6297,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="4" t="s">
         <v>42</v>
       </c>
@@ -6294,7 +6305,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="4" t="s">
         <v>42</v>
       </c>
@@ -6302,7 +6313,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="4" t="s">
         <v>42</v>
       </c>
@@ -6310,7 +6321,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="4" t="s">
         <v>42</v>
       </c>
@@ -6318,7 +6329,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="4" t="s">
         <v>42</v>
       </c>
@@ -6326,7 +6337,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="4" t="s">
         <v>42</v>
       </c>
@@ -6334,7 +6345,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="4" t="s">
         <v>54</v>
       </c>
@@ -6342,7 +6353,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="4" t="s">
         <v>54</v>
       </c>
@@ -6350,7 +6361,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="4" t="s">
         <v>54</v>
       </c>
@@ -6358,7 +6369,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="4" t="s">
         <v>54</v>
       </c>
@@ -6366,7 +6377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="4" t="s">
         <v>57</v>
       </c>
@@ -6374,7 +6385,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="4" t="s">
         <v>57</v>
       </c>
@@ -6382,7 +6393,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="4" t="s">
         <v>57</v>
       </c>
@@ -6390,7 +6401,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33" s="4" t="s">
         <v>57</v>
       </c>
@@ -6398,7 +6409,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34" s="4" t="s">
         <v>57</v>
       </c>
@@ -6406,7 +6417,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35" s="4" t="s">
         <v>170</v>
       </c>
@@ -6414,7 +6425,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H36" s="4" t="s">
         <v>170</v>
       </c>
@@ -6422,7 +6433,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H37" s="4" t="s">
         <v>170</v>
       </c>
@@ -6430,7 +6441,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H38" s="4" t="s">
         <v>170</v>
       </c>
@@ -6438,7 +6449,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="4" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
#1134 - Complex Actions
added action handlers for following:
  - AddEvent
  - AddPhase
  - CreateWork
  - SetEventDate
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935D0CA8-2159-46F6-A5C5-4F6BE19AA8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EDB628-0284-40A7-BB40-B17873451F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Lookups" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Events!$A$1:$M$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,8 +36,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="202">
   <si>
     <t>Cell Colors</t>
   </si>
@@ -814,10 +812,16 @@
     <t>{"start_date_locked": true}</t>
   </si>
   <si>
-    <t>{"phase_name":"Project Notification Review","work_type_id": 1, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Project Notification", "start_at": 14 }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Project Notification Review","work_type_id": 1, "ea_act_id": 3, "event_name": "\"Draft\" Project Notification Initial Review", "start_at": 21 }</t>
+    <t>{"phase_name":"Project Notification Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "Submission of \"Draft\" Project Notification", "start_at": 14 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Project Notification Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "\"Draft\" Project Notification Initial Review", "start_at": 21 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Project Notification Review","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Project Notification Review", "legislated": false }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Project Notification Decision","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Project Notification Decision", "legislated": false }</t>
   </si>
 </sst>
 </file>
@@ -1381,55 +1385,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1450,18 +1454,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1491,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1513,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1539,7 +1543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1565,226 +1569,226 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93"/>
     </row>
   </sheetData>
@@ -1824,25 +1828,25 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1922,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1961,7 +1965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2000,7 +2004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2039,7 +2043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2078,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2117,7 +2121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2156,7 +2160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2195,7 +2199,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2234,7 +2238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2273,7 +2277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2315,7 +2319,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2357,7 +2361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2399,7 +2403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2480,7 +2484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2519,7 +2523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2561,7 +2565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2600,7 +2604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2642,7 +2646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2684,7 +2688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2726,7 +2730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2768,7 +2772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2807,7 +2811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2885,7 +2889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2927,7 +2931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2969,7 +2973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3008,7 +3012,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3050,7 +3054,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3092,7 +3096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3131,7 +3135,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3173,7 +3177,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3215,7 +3219,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3254,7 +3258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3296,7 +3300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3338,7 +3342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3377,7 +3381,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3419,7 +3423,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3461,7 +3465,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3584,7 +3588,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3623,7 +3627,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3662,7 +3666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3701,7 +3705,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3740,7 +3744,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3782,7 +3786,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3821,7 +3825,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3860,7 +3864,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3902,7 +3906,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3944,7 +3948,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3983,7 +3987,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4025,7 +4029,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4067,7 +4071,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4106,7 +4110,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4148,7 +4152,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4190,7 +4194,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4229,7 +4233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4271,7 +4275,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4313,7 +4317,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4352,7 +4356,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4394,7 +4398,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4436,7 +4440,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4475,7 +4479,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4514,7 +4518,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4556,7 +4560,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4656,19 +4660,19 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4685,7 +4689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4703,7 +4707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4721,7 +4725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4739,7 +4743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4757,7 +4761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4775,7 +4779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4793,7 +4797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4811,7 +4815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4829,7 +4833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4847,7 +4851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4865,7 +4869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4883,7 +4887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4901,7 +4905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4919,7 +4923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4959,25 +4963,25 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="176.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="141.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="176.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="141.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -5000,7 +5004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5024,7 +5028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -5048,7 +5052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -5072,7 +5076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -5096,7 +5100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -5120,7 +5124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -5144,7 +5148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5168,7 +5172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5192,7 +5196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -5216,7 +5220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -5240,7 +5244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -5264,7 +5268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -5288,7 +5292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -5312,7 +5316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -5336,7 +5340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -5360,7 +5364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -5384,7 +5388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -5408,7 +5412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -5432,7 +5436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -5456,7 +5460,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -5480,7 +5484,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5504,7 +5508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5528,7 +5532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -5552,7 +5556,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -5576,7 +5580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -5600,7 +5604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -5618,13 +5622,13 @@
         <v>151</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -5642,13 +5646,13 @@
         <v>152</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -5672,7 +5676,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -5696,7 +5700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -5720,7 +5724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -5744,7 +5748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5768,7 +5772,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5792,7 +5796,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5816,7 +5820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -5840,7 +5844,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -5864,7 +5868,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -5888,20 +5892,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G34" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}"/>
+  <autoFilter ref="A1:G38" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -5927,34 +5931,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.88671875" style="4"/>
-    <col min="60" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.85546875" style="4"/>
+    <col min="60" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -6033,7 +6037,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -6065,7 +6069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>161</v>
       </c>
@@ -6097,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>164</v>
       </c>
@@ -6120,7 +6124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>168</v>
       </c>
@@ -6137,7 +6141,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>172</v>
       </c>
@@ -6154,7 +6158,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>174</v>
       </c>
@@ -6171,7 +6175,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>176</v>
       </c>
@@ -6188,7 +6192,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>179</v>
       </c>
@@ -6202,7 +6206,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>181</v>
       </c>
@@ -6214,7 +6218,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>182</v>
       </c>
@@ -6226,7 +6230,7 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>183</v>
       </c>
@@ -6238,7 +6242,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>184</v>
       </c>
@@ -6250,7 +6254,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>185</v>
       </c>
@@ -6262,7 +6266,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
@@ -6273,7 +6277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="4" t="s">
         <v>42</v>
       </c>
@@ -6281,7 +6285,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="4" t="s">
         <v>42</v>
       </c>
@@ -6289,7 +6293,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="4" t="s">
         <v>42</v>
       </c>
@@ -6297,7 +6301,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="4" t="s">
         <v>42</v>
       </c>
@@ -6305,7 +6309,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="4" t="s">
         <v>42</v>
       </c>
@@ -6313,7 +6317,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="4" t="s">
         <v>42</v>
       </c>
@@ -6321,7 +6325,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="4" t="s">
         <v>42</v>
       </c>
@@ -6329,7 +6333,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H24" s="4" t="s">
         <v>42</v>
       </c>
@@ -6337,7 +6341,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H25" s="4" t="s">
         <v>42</v>
       </c>
@@ -6345,7 +6349,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H26" s="4" t="s">
         <v>54</v>
       </c>
@@ -6353,7 +6357,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="4" t="s">
         <v>54</v>
       </c>
@@ -6361,7 +6365,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H28" s="4" t="s">
         <v>54</v>
       </c>
@@ -6369,7 +6373,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H29" s="4" t="s">
         <v>54</v>
       </c>
@@ -6377,7 +6381,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H30" s="4" t="s">
         <v>57</v>
       </c>
@@ -6385,7 +6389,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H31" s="4" t="s">
         <v>57</v>
       </c>
@@ -6393,7 +6397,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H32" s="4" t="s">
         <v>57</v>
       </c>
@@ -6401,7 +6405,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="4" t="s">
         <v>57</v>
       </c>
@@ -6409,7 +6413,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="4" t="s">
         <v>57</v>
       </c>
@@ -6417,7 +6421,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" s="4" t="s">
         <v>170</v>
       </c>
@@ -6425,7 +6429,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36" s="4" t="s">
         <v>170</v>
       </c>
@@ -6433,7 +6437,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37" s="4" t="s">
         <v>170</v>
       </c>
@@ -6441,7 +6445,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38" s="4" t="s">
         <v>170</v>
       </c>
@@ -6449,7 +6453,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39" s="4" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
project notification template updated + master templates added
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\project_notification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E6729C-7842-4851-B78E-87FC8953B47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A2E1EA-F9B0-46DA-86D9-7E19AB94FE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Lookups" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Events!$A$1:$M$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="201">
   <si>
     <t>Cell Colors</t>
   </si>
@@ -549,9 +549,6 @@
   </si>
   <si>
     <t>CEAO is delegated to make the final Project Notification Decision</t>
-  </si>
-  <si>
-    <t>Days are added to the PHASE END EVENT</t>
   </si>
   <si>
     <t>Project Notification is Terminated under s.39(d) of Act</t>
@@ -1385,55 +1382,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1454,18 +1451,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1517,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1543,7 +1540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1569,226 +1566,226 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93"/>
     </row>
   </sheetData>
@@ -1824,29 +1821,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1872,7 +1869,7 @@
         <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -1887,7 +1884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1926,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1965,7 +1962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2004,7 +2001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2043,7 +2040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2082,7 +2079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2121,7 +2118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2160,7 +2157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2199,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2238,7 +2235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2277,7 +2274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2319,7 +2316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2361,7 +2358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2403,7 +2400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2445,7 +2442,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2484,7 +2481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2523,7 +2520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2565,7 +2562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2604,7 +2601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2646,7 +2643,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2688,7 +2685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2730,7 +2727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2772,7 +2769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2850,7 +2847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2889,7 +2886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2931,7 +2928,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2973,7 +2970,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3012,7 +3009,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3054,7 +3051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3096,7 +3093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3135,7 +3132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3177,7 +3174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3219,7 +3216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3258,7 +3255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3300,7 +3297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3342,7 +3339,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3381,7 +3378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3423,7 +3420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3465,7 +3462,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3504,7 +3501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3546,7 +3543,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3588,7 +3585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3627,7 +3624,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3666,7 +3663,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3705,7 +3702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3744,7 +3741,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3786,7 +3783,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3825,7 +3822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3864,7 +3861,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3906,7 +3903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3948,7 +3945,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3987,7 +3984,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4029,7 +4026,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4071,7 +4068,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4110,7 +4107,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4152,7 +4149,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4194,7 +4191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4233,7 +4230,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4275,7 +4272,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4317,7 +4314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4356,7 +4353,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4398,7 +4395,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4440,7 +4437,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4479,7 +4476,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4518,7 +4515,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4560,7 +4557,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4654,25 +4651,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E0C025-141A-44A8-A6E5-45461DB42BA4}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4689,7 +4686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4707,7 +4704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4725,7 +4722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4743,7 +4740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4761,7 +4758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4779,7 +4776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4797,61 +4794,61 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="8">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6" t="str">
         <f>IF((B8=""),"",VLOOKUP(B8,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>s.38 Extension of Time Limit</v>
+        <v>Project Notification Terminated s.39(d)</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E8" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="8">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="str">
         <f>IF((B9=""),"",VLOOKUP(B9,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Notification Terminated s.39(d)</v>
+        <v>Project Withdrawn</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E9" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="8">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C10" s="6" t="str">
         <f>IF((B10=""),"",VLOOKUP(B10,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Withdrawn</v>
+        <v>Decision: Project Notification</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E10" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4866,10 +4863,10 @@
         <v>113</v>
       </c>
       <c r="E11" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4884,60 +4881,42 @@
         <v>114</v>
       </c>
       <c r="E12" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="8">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C13" s="6" t="str">
         <f>IF((B13=""),"",VLOOKUP(B13,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Decision: Project Notification</v>
+        <v>Project Notification Terminated s.39(d)</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E13" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="8">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C14" s="6" t="str">
         <f>IF((B14=""),"",VLOOKUP(B14,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Notification Terminated s.39(d)</v>
+        <v>Project Withdrawn</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E14" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8">
-        <v>61</v>
-      </c>
-      <c r="C15" s="6" t="str">
-        <f>IF((B15=""),"",VLOOKUP(B15,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Withdrawn</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="3">
         <v>14</v>
       </c>
     </row>
@@ -4950,7 +4929,7 @@
           <x14:formula1>
             <xm:f>Events!$A$2:$A$68</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B15</xm:sqref>
+          <xm:sqref>B2:B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4960,51 +4939,51 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="176.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="141.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="176.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="141.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5012,23 +4991,23 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="str">
-        <f>IF((B2=""),"",VLOOKUP(B2,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B2=""),"",VLOOKUP(B2,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Initial Review of "Draft" Project Notification is POSITIVE</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -5036,23 +5015,23 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="str">
-        <f>IF((B3=""),"",VLOOKUP(B3,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B3=""),"",VLOOKUP(B3,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Initial Review of "Draft" Project Notification is NEGATIVE</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -5060,23 +5039,23 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="str">
-        <f>IF((B4=""),"",VLOOKUP(B4,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B4=""),"",VLOOKUP(B4,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Initial Review of "Draft" Project Notification is NEGATIVE</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -5084,23 +5063,23 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="str">
-        <f>IF((B5=""),"",VLOOKUP(B5,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B5=""),"",VLOOKUP(B5,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -5108,23 +5087,23 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="str">
-        <f>IF((B6=""),"",VLOOKUP(B6,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B6=""),"",VLOOKUP(B6,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -5132,23 +5111,23 @@
         <v>3</v>
       </c>
       <c r="C7" s="6" t="str">
-        <f>IF((B7=""),"",VLOOKUP(B7,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B7=""),"",VLOOKUP(B7,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5156,23 +5135,23 @@
         <v>3</v>
       </c>
       <c r="C8" s="6" t="str">
-        <f>IF((B8=""),"",VLOOKUP(B8,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B8=""),"",VLOOKUP(B8,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5180,23 +5159,23 @@
         <v>4</v>
       </c>
       <c r="C9" s="6" t="str">
-        <f>IF((B9=""),"",VLOOKUP(B9,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B9=""),"",VLOOKUP(B9,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Starts the "clock" for Project Notification</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -5204,23 +5183,23 @@
         <v>5</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f>IF((B10=""),"",VLOOKUP(B10,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B10=""),"",VLOOKUP(B10,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Minister is delegated to make the final Project Notification Decision</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -5228,693 +5207,597 @@
         <v>6</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>IF((B11=""),"",VLOOKUP(B11,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B11=""),"",VLOOKUP(B11,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>CEAO is delegated to make the final Project Notification Decision</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" s="8">
         <v>7</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>IF((B12=""),"",VLOOKUP(B12,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B12=""),"",VLOOKUP(B12,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="G12" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B13" s="8">
         <v>7</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f>IF((B13=""),"",VLOOKUP(B13,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B13=""),"",VLOOKUP(B13,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G13" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="8">
         <v>7</v>
       </c>
       <c r="C14" s="6" t="str">
-        <f>IF((B14=""),"",VLOOKUP(B14,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B14=""),"",VLOOKUP(B14,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="G14" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="8">
         <v>7</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f>IF((B15=""),"",VLOOKUP(B15,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B15=""),"",VLOOKUP(B15,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G15" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" s="8">
         <v>8</v>
       </c>
       <c r="C16" s="6" t="str">
-        <f>IF((B16=""),"",VLOOKUP(B16,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B16=""),"",VLOOKUP(B16,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="G16" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" s="8">
         <v>8</v>
       </c>
       <c r="C17" s="6" t="str">
-        <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G17" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18" s="8">
         <v>8</v>
       </c>
       <c r="C18" s="6" t="str">
-        <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="G18" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" s="8">
         <v>8</v>
       </c>
       <c r="C19" s="6" t="str">
-        <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G19" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" s="8">
         <v>9</v>
       </c>
       <c r="C20" s="6" t="str">
-        <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>No Further Review Required</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="G20" s="3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B21" s="8">
         <v>9</v>
       </c>
       <c r="C21" s="6" t="str">
-        <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>No Further Review Required</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G21" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="6" t="str">
-        <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>More Information Needed</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="G22" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="6" t="str">
-        <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>More Information Needed</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
       <c r="G23" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24" s="8">
         <v>10</v>
       </c>
       <c r="C24" s="6" t="str">
-        <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>No Further Review Required</v>
+        <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>More Information Needed</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G24" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="6" t="str">
-        <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>No Further Review Required</v>
+        <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Referred to Minister (s.11)</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="G25" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="8">
         <v>11</v>
       </c>
       <c r="C26" s="6" t="str">
-        <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>More Information Needed</v>
+        <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Referred to Minister (s.11)</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="G26" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="6" t="str">
-        <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>More Information Needed</v>
+        <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>199</v>
+        <v>127</v>
       </c>
       <c r="G27" s="3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B28" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28" s="6" t="str">
-        <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>More Information Needed</v>
+        <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>200</v>
+        <v>127</v>
       </c>
       <c r="G28" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B29" s="8">
         <v>12</v>
       </c>
       <c r="C29" s="6" t="str">
-        <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Referred to Minister (s.11)</v>
+        <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="G29" s="3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B30" s="8">
         <v>12</v>
       </c>
       <c r="C30" s="6" t="str">
-        <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Referred to Minister (s.11)</v>
+        <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G30" s="3">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B31" s="8">
         <v>13</v>
       </c>
       <c r="C31" s="6" t="str">
-        <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="G31" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B32" s="8">
         <v>13</v>
       </c>
       <c r="C32" s="6" t="str">
-        <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G32" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="8">
         <v>13</v>
       </c>
       <c r="C33" s="6" t="str">
-        <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="G33" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B34" s="8">
         <v>13</v>
       </c>
       <c r="C34" s="6" t="str">
-        <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G34" s="3">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>34</v>
-      </c>
-      <c r="B35" s="8">
-        <v>14</v>
-      </c>
-      <c r="C35" s="6" t="str">
-        <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G35" s="3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>35</v>
-      </c>
-      <c r="B36" s="8">
-        <v>14</v>
-      </c>
-      <c r="C36" s="6" t="str">
-        <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G36" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="8">
-        <v>14</v>
-      </c>
-      <c r="C37" s="6" t="str">
-        <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G37" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="8">
-        <v>14</v>
-      </c>
-      <c r="C38" s="6" t="str">
-        <f>IF((B38=""),"",VLOOKUP(B38,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D39"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D42"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G38" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}"/>
+  <autoFilter ref="A1:G34" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD376E2D-0D02-46B5-8EB4-1C59799E70C5}">
           <x14:formula1>
-            <xm:f>Outcomes!$A$2:$A$15</xm:f>
+            <xm:f>Outcomes!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B38</xm:sqref>
+          <xm:sqref>B2:B34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5931,41 +5814,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.85546875" style="4"/>
-    <col min="60" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.88671875" style="4"/>
+    <col min="60" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1" t="s">
@@ -5974,11 +5857,11 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="1" t="s">
@@ -5986,15 +5869,15 @@
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -6037,7 +5920,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -6060,7 +5943,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>35</v>
@@ -6069,12 +5952,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="F4" s="2" t="b">
         <v>0</v>
@@ -6092,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>38</v>
@@ -6101,49 +5984,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>41</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>34</v>
@@ -6155,12 +6038,12 @@
         <v>53</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>34</v>
@@ -6172,29 +6055,29 @@
         <v>75</v>
       </c>
       <c r="O8" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>80</v>
       </c>
       <c r="O9" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>34</v>
@@ -6203,12 +6086,12 @@
         <v>37</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>34</v>
@@ -6218,9 +6101,9 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>34</v>
@@ -6230,9 +6113,9 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>75</v>
@@ -6242,9 +6125,9 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>75</v>
@@ -6254,9 +6137,9 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>80</v>
@@ -6266,7 +6149,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
@@ -6277,15 +6160,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="4" t="s">
         <v>41</v>
       </c>
@@ -6293,7 +6176,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="4" t="s">
         <v>41</v>
       </c>
@@ -6301,15 +6184,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="4" t="s">
         <v>41</v>
       </c>
@@ -6317,7 +6200,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="4" t="s">
         <v>41</v>
       </c>
@@ -6325,23 +6208,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="4" t="s">
         <v>41</v>
       </c>
@@ -6349,7 +6232,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="4" t="s">
         <v>53</v>
       </c>
@@ -6357,7 +6240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="4" t="s">
         <v>53</v>
       </c>
@@ -6365,7 +6248,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="4" t="s">
         <v>53</v>
       </c>
@@ -6373,7 +6256,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="4" t="s">
         <v>53</v>
       </c>
@@ -6381,7 +6264,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="4" t="s">
         <v>56</v>
       </c>
@@ -6389,7 +6272,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="4" t="s">
         <v>56</v>
       </c>
@@ -6397,23 +6280,23 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34" s="4" t="s">
         <v>56</v>
       </c>
@@ -6421,41 +6304,41 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H36" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H36" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I36" s="2" t="s">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H37" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H37" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I37" s="2" t="s">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H38" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
project notification template updated + master templates added (#1183)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/001-Project_Notification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\project_notification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E6729C-7842-4851-B78E-87FC8953B47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A2E1EA-F9B0-46DA-86D9-7E19AB94FE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Lookups" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Actions!$A$1:$G$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Events!$A$1:$M$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="201">
   <si>
     <t>Cell Colors</t>
   </si>
@@ -549,9 +549,6 @@
   </si>
   <si>
     <t>CEAO is delegated to make the final Project Notification Decision</t>
-  </si>
-  <si>
-    <t>Days are added to the PHASE END EVENT</t>
   </si>
   <si>
     <t>Project Notification is Terminated under s.39(d) of Act</t>
@@ -1385,55 +1382,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1454,18 +1451,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1517,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1543,7 +1540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1569,226 +1566,226 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93"/>
     </row>
   </sheetData>
@@ -1824,29 +1821,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1872,7 +1869,7 @@
         <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -1887,7 +1884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1926,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1965,7 +1962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2004,7 +2001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2043,7 +2040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2082,7 +2079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2121,7 +2118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2160,7 +2157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2199,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2238,7 +2235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2277,7 +2274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2319,7 +2316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2361,7 +2358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2403,7 +2400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2445,7 +2442,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2484,7 +2481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2523,7 +2520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2565,7 +2562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2604,7 +2601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2646,7 +2643,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2688,7 +2685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2730,7 +2727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2772,7 +2769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2850,7 +2847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2889,7 +2886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2931,7 +2928,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2973,7 +2970,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3012,7 +3009,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3054,7 +3051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3096,7 +3093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3135,7 +3132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3177,7 +3174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3219,7 +3216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3258,7 +3255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3300,7 +3297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3342,7 +3339,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3381,7 +3378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3423,7 +3420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3465,7 +3462,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3504,7 +3501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3546,7 +3543,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3588,7 +3585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3627,7 +3624,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3666,7 +3663,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3705,7 +3702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3744,7 +3741,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3786,7 +3783,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3825,7 +3822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3864,7 +3861,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3906,7 +3903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3948,7 +3945,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3987,7 +3984,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4029,7 +4026,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4071,7 +4068,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4110,7 +4107,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4152,7 +4149,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4194,7 +4191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4233,7 +4230,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4275,7 +4272,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4317,7 +4314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4356,7 +4353,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4398,7 +4395,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4440,7 +4437,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4479,7 +4476,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4518,7 +4515,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4560,7 +4557,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4654,25 +4651,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E0C025-141A-44A8-A6E5-45461DB42BA4}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4689,7 +4686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4707,7 +4704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4725,7 +4722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4743,7 +4740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4761,7 +4758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4779,7 +4776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4797,61 +4794,61 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="8">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6" t="str">
         <f>IF((B8=""),"",VLOOKUP(B8,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>s.38 Extension of Time Limit</v>
+        <v>Project Notification Terminated s.39(d)</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E8" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="8">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="str">
         <f>IF((B9=""),"",VLOOKUP(B9,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Notification Terminated s.39(d)</v>
+        <v>Project Withdrawn</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E9" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="8">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C10" s="6" t="str">
         <f>IF((B10=""),"",VLOOKUP(B10,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Withdrawn</v>
+        <v>Decision: Project Notification</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E10" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4866,10 +4863,10 @@
         <v>113</v>
       </c>
       <c r="E11" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4884,60 +4881,42 @@
         <v>114</v>
       </c>
       <c r="E12" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="8">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C13" s="6" t="str">
         <f>IF((B13=""),"",VLOOKUP(B13,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Decision: Project Notification</v>
+        <v>Project Notification Terminated s.39(d)</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E13" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="8">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C14" s="6" t="str">
         <f>IF((B14=""),"",VLOOKUP(B14,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Notification Terminated s.39(d)</v>
+        <v>Project Withdrawn</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E14" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8">
-        <v>61</v>
-      </c>
-      <c r="C15" s="6" t="str">
-        <f>IF((B15=""),"",VLOOKUP(B15,Events!$A$2:$D$68,4,FALSE))</f>
-        <v>Project Withdrawn</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="3">
         <v>14</v>
       </c>
     </row>
@@ -4950,7 +4929,7 @@
           <x14:formula1>
             <xm:f>Events!$A$2:$A$68</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B15</xm:sqref>
+          <xm:sqref>B2:B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4960,51 +4939,51 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="176.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="141.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="176.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="141.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5012,23 +4991,23 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="str">
-        <f>IF((B2=""),"",VLOOKUP(B2,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B2=""),"",VLOOKUP(B2,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Initial Review of "Draft" Project Notification is POSITIVE</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -5036,23 +5015,23 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="str">
-        <f>IF((B3=""),"",VLOOKUP(B3,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B3=""),"",VLOOKUP(B3,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Initial Review of "Draft" Project Notification is NEGATIVE</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -5060,23 +5039,23 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="str">
-        <f>IF((B4=""),"",VLOOKUP(B4,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B4=""),"",VLOOKUP(B4,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Initial Review of "Draft" Project Notification is NEGATIVE</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -5084,23 +5063,23 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="str">
-        <f>IF((B5=""),"",VLOOKUP(B5,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B5=""),"",VLOOKUP(B5,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -5108,23 +5087,23 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="str">
-        <f>IF((B6=""),"",VLOOKUP(B6,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B6=""),"",VLOOKUP(B6,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -5132,23 +5111,23 @@
         <v>3</v>
       </c>
       <c r="C7" s="6" t="str">
-        <f>IF((B7=""),"",VLOOKUP(B7,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B7=""),"",VLOOKUP(B7,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5156,23 +5135,23 @@
         <v>3</v>
       </c>
       <c r="C8" s="6" t="str">
-        <f>IF((B8=""),"",VLOOKUP(B8,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B8=""),"",VLOOKUP(B8,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5180,23 +5159,23 @@
         <v>4</v>
       </c>
       <c r="C9" s="6" t="str">
-        <f>IF((B9=""),"",VLOOKUP(B9,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B9=""),"",VLOOKUP(B9,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Starts the "clock" for Project Notification</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -5204,23 +5183,23 @@
         <v>5</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f>IF((B10=""),"",VLOOKUP(B10,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B10=""),"",VLOOKUP(B10,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>Minister is delegated to make the final Project Notification Decision</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -5228,693 +5207,597 @@
         <v>6</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>IF((B11=""),"",VLOOKUP(B11,Outcomes!$A$2:$D$15,4,FALSE))</f>
+        <f>IF((B11=""),"",VLOOKUP(B11,Outcomes!$A$2:$D$14,4,FALSE))</f>
         <v>CEAO is delegated to make the final Project Notification Decision</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" s="8">
         <v>7</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>IF((B12=""),"",VLOOKUP(B12,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B12=""),"",VLOOKUP(B12,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="G12" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B13" s="8">
         <v>7</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f>IF((B13=""),"",VLOOKUP(B13,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B13=""),"",VLOOKUP(B13,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G13" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="8">
         <v>7</v>
       </c>
       <c r="C14" s="6" t="str">
-        <f>IF((B14=""),"",VLOOKUP(B14,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B14=""),"",VLOOKUP(B14,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="G14" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="8">
         <v>7</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f>IF((B15=""),"",VLOOKUP(B15,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Days are added to the PHASE END EVENT</v>
+        <f>IF((B15=""),"",VLOOKUP(B15,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G15" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" s="8">
         <v>8</v>
       </c>
       <c r="C16" s="6" t="str">
-        <f>IF((B16=""),"",VLOOKUP(B16,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B16=""),"",VLOOKUP(B16,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="G16" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" s="8">
         <v>8</v>
       </c>
       <c r="C17" s="6" t="str">
-        <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G17" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18" s="8">
         <v>8</v>
       </c>
       <c r="C18" s="6" t="str">
-        <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="G18" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" s="8">
         <v>8</v>
       </c>
       <c r="C19" s="6" t="str">
-        <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G19" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" s="8">
         <v>9</v>
       </c>
       <c r="C20" s="6" t="str">
-        <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>No Further Review Required</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="G20" s="3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B21" s="8">
         <v>9</v>
       </c>
       <c r="C21" s="6" t="str">
-        <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>No Further Review Required</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G21" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="6" t="str">
-        <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>More Information Needed</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="G22" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="6" t="str">
-        <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
+        <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>More Information Needed</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
       <c r="G23" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24" s="8">
         <v>10</v>
       </c>
       <c r="C24" s="6" t="str">
-        <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>No Further Review Required</v>
+        <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>More Information Needed</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G24" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="6" t="str">
-        <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>No Further Review Required</v>
+        <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Referred to Minister (s.11)</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="G25" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="8">
         <v>11</v>
       </c>
       <c r="C26" s="6" t="str">
-        <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>More Information Needed</v>
+        <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Referred to Minister (s.11)</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="G26" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="6" t="str">
-        <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>More Information Needed</v>
+        <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>199</v>
+        <v>127</v>
       </c>
       <c r="G27" s="3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B28" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28" s="6" t="str">
-        <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>More Information Needed</v>
+        <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>200</v>
+        <v>127</v>
       </c>
       <c r="G28" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B29" s="8">
         <v>12</v>
       </c>
       <c r="C29" s="6" t="str">
-        <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Referred to Minister (s.11)</v>
+        <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="G29" s="3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B30" s="8">
         <v>12</v>
       </c>
       <c r="C30" s="6" t="str">
-        <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Referred to Minister (s.11)</v>
+        <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Project Notification is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G30" s="3">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B31" s="8">
         <v>13</v>
       </c>
       <c r="C31" s="6" t="str">
-        <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="G31" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B32" s="8">
         <v>13</v>
       </c>
       <c r="C32" s="6" t="str">
-        <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G32" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="8">
         <v>13</v>
       </c>
       <c r="C33" s="6" t="str">
-        <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="G33" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B34" s="8">
         <v>13</v>
       </c>
       <c r="C34" s="6" t="str">
-        <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Project Notification is Terminated under s.39(d) of Act</v>
+        <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$14,4,FALSE))</f>
+        <v>Proponent withdraws Submission from the Project Notification process</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G34" s="3">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>34</v>
-      </c>
-      <c r="B35" s="8">
-        <v>14</v>
-      </c>
-      <c r="C35" s="6" t="str">
-        <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G35" s="3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>35</v>
-      </c>
-      <c r="B36" s="8">
-        <v>14</v>
-      </c>
-      <c r="C36" s="6" t="str">
-        <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G36" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="8">
-        <v>14</v>
-      </c>
-      <c r="C37" s="6" t="str">
-        <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G37" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="8">
-        <v>14</v>
-      </c>
-      <c r="C38" s="6" t="str">
-        <f>IF((B38=""),"",VLOOKUP(B38,Outcomes!$A$2:$D$15,4,FALSE))</f>
-        <v>Proponent withdraws Submission from the Project Notification process</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D39"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D42"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G38" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}"/>
+  <autoFilter ref="A1:G34" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD376E2D-0D02-46B5-8EB4-1C59799E70C5}">
           <x14:formula1>
-            <xm:f>Outcomes!$A$2:$A$15</xm:f>
+            <xm:f>Outcomes!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B38</xm:sqref>
+          <xm:sqref>B2:B34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5931,41 +5814,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.85546875" style="4"/>
-    <col min="60" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.88671875" style="4"/>
+    <col min="60" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1" t="s">
@@ -5974,11 +5857,11 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="1" t="s">
@@ -5986,15 +5869,15 @@
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -6037,7 +5920,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -6060,7 +5943,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>35</v>
@@ -6069,12 +5952,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="F4" s="2" t="b">
         <v>0</v>
@@ -6092,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>38</v>
@@ -6101,49 +5984,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>41</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>34</v>
@@ -6155,12 +6038,12 @@
         <v>53</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>34</v>
@@ -6172,29 +6055,29 @@
         <v>75</v>
       </c>
       <c r="O8" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>80</v>
       </c>
       <c r="O9" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>34</v>
@@ -6203,12 +6086,12 @@
         <v>37</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>34</v>
@@ -6218,9 +6101,9 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>34</v>
@@ -6230,9 +6113,9 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>75</v>
@@ -6242,9 +6125,9 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>75</v>
@@ -6254,9 +6137,9 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>80</v>
@@ -6266,7 +6149,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
@@ -6277,15 +6160,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="4" t="s">
         <v>41</v>
       </c>
@@ -6293,7 +6176,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="4" t="s">
         <v>41</v>
       </c>
@@ -6301,15 +6184,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="4" t="s">
         <v>41</v>
       </c>
@@ -6317,7 +6200,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="4" t="s">
         <v>41</v>
       </c>
@@ -6325,23 +6208,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="4" t="s">
         <v>41</v>
       </c>
@@ -6349,7 +6232,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="4" t="s">
         <v>53</v>
       </c>
@@ -6357,7 +6240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="4" t="s">
         <v>53</v>
       </c>
@@ -6365,7 +6248,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="4" t="s">
         <v>53</v>
       </c>
@@ -6373,7 +6256,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="4" t="s">
         <v>53</v>
       </c>
@@ -6381,7 +6264,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="4" t="s">
         <v>56</v>
       </c>
@@ -6389,7 +6272,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="4" t="s">
         <v>56</v>
       </c>
@@ -6397,23 +6280,23 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34" s="4" t="s">
         <v>56</v>
       </c>
@@ -6421,41 +6304,41 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H36" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H36" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I36" s="2" t="s">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H37" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H37" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I37" s="2" t="s">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H38" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>45</v>

</xml_diff>